<commit_message>
Updated the spreadsheets with new tests
</commit_message>
<xml_diff>
--- a/daffodil-core/doc/Test_Cases.xlsx
+++ b/daffodil-core/doc/Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="27795" windowHeight="11580"/>
+    <workbookView xWindow="480" yWindow="396" windowWidth="27792" windowHeight="11520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="159">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -418,6 +418,81 @@
   </si>
   <si>
     <t>ParseSequence5</t>
+  </si>
+  <si>
+    <t>property_scoping_02</t>
+  </si>
+  <si>
+    <t>DFDL-8-018R</t>
+  </si>
+  <si>
+    <t>DFDL-69/DFDL-70</t>
+  </si>
+  <si>
+    <t>DFDL-7-028R</t>
+  </si>
+  <si>
+    <t>defineFormat_01</t>
+  </si>
+  <si>
+    <t>property_scoping_04</t>
+  </si>
+  <si>
+    <t>DFDL-8-022R</t>
+  </si>
+  <si>
+    <t>DFDL-8-021R</t>
+  </si>
+  <si>
+    <t>DFDL-69/DFDL-71</t>
+  </si>
+  <si>
+    <t>property_scoping_05</t>
+  </si>
+  <si>
+    <t>DFDL-69/DFDL-72, DFDL-131</t>
+  </si>
+  <si>
+    <t>escapeSchemeSimple</t>
+  </si>
+  <si>
+    <t>DFDL-7-079R</t>
+  </si>
+  <si>
+    <t>DFDL-269</t>
+  </si>
+  <si>
+    <t>DelimProp_04</t>
+  </si>
+  <si>
+    <t>DelimProp_02</t>
+  </si>
+  <si>
+    <t>SeqGrp_02</t>
+  </si>
+  <si>
+    <t>SeqGrp_03</t>
+  </si>
+  <si>
+    <t>DelimProp_09</t>
+  </si>
+  <si>
+    <t>DelimProp_10</t>
+  </si>
+  <si>
+    <t>SeqGrp_04</t>
+  </si>
+  <si>
+    <t>ParseSequence_4a</t>
+  </si>
+  <si>
+    <t>AI000</t>
+  </si>
+  <si>
+    <t>DFDL-12-038R</t>
+  </si>
+  <si>
+    <t>DFDL-156</t>
   </si>
 </sst>
 </file>
@@ -783,23 +858,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
+      <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -831,7 +906,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -854,7 +929,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -877,7 +952,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -900,7 +975,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>15</v>
       </c>
@@ -923,7 +998,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -946,7 +1021,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -969,7 +1044,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -995,7 +1070,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -1018,7 +1093,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -1044,7 +1119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -1067,7 +1142,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>29</v>
       </c>
@@ -1093,7 +1168,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -1119,7 +1194,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1145,7 +1220,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>37</v>
       </c>
@@ -1171,7 +1246,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -1197,7 +1272,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>39</v>
       </c>
@@ -1223,7 +1298,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>41</v>
       </c>
@@ -1249,7 +1324,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>43</v>
       </c>
@@ -1275,7 +1350,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>45</v>
       </c>
@@ -1298,7 +1373,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>46</v>
       </c>
@@ -1321,7 +1396,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>49</v>
       </c>
@@ -1347,7 +1422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>50</v>
       </c>
@@ -1370,7 +1445,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>53</v>
       </c>
@@ -1393,7 +1468,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>54</v>
       </c>
@@ -1416,7 +1491,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>55</v>
       </c>
@@ -1439,7 +1514,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>57</v>
       </c>
@@ -1462,7 +1537,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>59</v>
       </c>
@@ -1485,7 +1560,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>62</v>
       </c>
@@ -1508,7 +1583,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>63</v>
       </c>
@@ -1531,7 +1606,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>64</v>
       </c>
@@ -1554,7 +1629,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>65</v>
       </c>
@@ -1577,7 +1652,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>66</v>
       </c>
@@ -1600,7 +1675,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>67</v>
       </c>
@@ -1623,7 +1698,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>68</v>
       </c>
@@ -1646,7 +1721,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>69</v>
       </c>
@@ -1669,7 +1744,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>70</v>
       </c>
@@ -1692,7 +1767,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>75</v>
       </c>
@@ -1715,7 +1790,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>76</v>
       </c>
@@ -1738,7 +1813,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>77</v>
       </c>
@@ -1761,7 +1836,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>78</v>
       </c>
@@ -1784,7 +1859,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>79</v>
       </c>
@@ -1807,7 +1882,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>82</v>
       </c>
@@ -1830,7 +1905,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>83</v>
       </c>
@@ -1853,7 +1928,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>86</v>
       </c>
@@ -1876,7 +1951,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>88</v>
       </c>
@@ -1899,7 +1974,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>90</v>
       </c>
@@ -1922,7 +1997,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>91</v>
       </c>
@@ -1945,7 +2020,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>92</v>
       </c>
@@ -1968,7 +2043,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>93</v>
       </c>
@@ -1991,7 +2066,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>94</v>
       </c>
@@ -2017,7 +2092,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>95</v>
       </c>
@@ -2040,7 +2115,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>96</v>
       </c>
@@ -2063,7 +2138,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>97</v>
       </c>
@@ -2086,7 +2161,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>100</v>
       </c>
@@ -2109,7 +2184,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>104</v>
       </c>
@@ -2132,7 +2207,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>106</v>
       </c>
@@ -2155,7 +2230,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>107</v>
       </c>
@@ -2178,7 +2253,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>109</v>
       </c>
@@ -2201,7 +2276,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>111</v>
       </c>
@@ -2224,7 +2299,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>112</v>
       </c>
@@ -2247,7 +2322,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>113</v>
       </c>
@@ -2270,7 +2345,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>114</v>
       </c>
@@ -2293,7 +2368,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" ht="15" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>115</v>
       </c>
@@ -2316,7 +2391,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>116</v>
       </c>
@@ -2339,7 +2414,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>118</v>
       </c>
@@ -2362,7 +2437,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>119</v>
       </c>
@@ -2385,7 +2460,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>120</v>
       </c>
@@ -2408,7 +2483,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>121</v>
       </c>
@@ -2431,7 +2506,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>122</v>
       </c>
@@ -2454,7 +2529,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>123</v>
       </c>
@@ -2477,7 +2552,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>126</v>
       </c>
@@ -2500,7 +2575,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>127</v>
       </c>
@@ -2523,7 +2598,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>128</v>
       </c>
@@ -2546,7 +2621,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>130</v>
       </c>
@@ -2569,7 +2644,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>132</v>
       </c>
@@ -2592,7 +2667,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>133</v>
       </c>
@@ -2613,6 +2688,331 @@
       </c>
       <c r="H77" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>134</v>
+      </c>
+      <c r="C78" t="s">
+        <v>28</v>
+      </c>
+      <c r="D78" t="s">
+        <v>135</v>
+      </c>
+      <c r="E78" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="5">
+        <v>3</v>
+      </c>
+      <c r="G78" t="s">
+        <v>11</v>
+      </c>
+      <c r="H78" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>138</v>
+      </c>
+      <c r="C79" t="s">
+        <v>28</v>
+      </c>
+      <c r="D79" t="s">
+        <v>137</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="5">
+        <v>3</v>
+      </c>
+      <c r="G79" t="s">
+        <v>11</v>
+      </c>
+      <c r="H79" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>139</v>
+      </c>
+      <c r="C80" t="s">
+        <v>28</v>
+      </c>
+      <c r="D80" t="s">
+        <v>141</v>
+      </c>
+      <c r="E80" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" s="5">
+        <v>3</v>
+      </c>
+      <c r="G80" t="s">
+        <v>103</v>
+      </c>
+      <c r="H80" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>143</v>
+      </c>
+      <c r="C81" t="s">
+        <v>28</v>
+      </c>
+      <c r="D81" t="s">
+        <v>140</v>
+      </c>
+      <c r="E81" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="5">
+        <v>3</v>
+      </c>
+      <c r="G81" t="s">
+        <v>103</v>
+      </c>
+      <c r="H81" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>145</v>
+      </c>
+      <c r="C82" t="s">
+        <v>28</v>
+      </c>
+      <c r="D82" t="s">
+        <v>146</v>
+      </c>
+      <c r="E82" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="5">
+        <v>3</v>
+      </c>
+      <c r="G82" t="s">
+        <v>11</v>
+      </c>
+      <c r="H82" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>148</v>
+      </c>
+      <c r="C83" t="s">
+        <v>28</v>
+      </c>
+      <c r="D83" t="s">
+        <v>56</v>
+      </c>
+      <c r="E83" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="5">
+        <v>3</v>
+      </c>
+      <c r="G83" t="s">
+        <v>11</v>
+      </c>
+      <c r="H83" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>149</v>
+      </c>
+      <c r="C84" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84" t="s">
+        <v>56</v>
+      </c>
+      <c r="E84" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="5">
+        <v>3</v>
+      </c>
+      <c r="G84" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>150</v>
+      </c>
+      <c r="C85" t="s">
+        <v>28</v>
+      </c>
+      <c r="D85" t="s">
+        <v>84</v>
+      </c>
+      <c r="E85" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" s="5">
+        <v>3</v>
+      </c>
+      <c r="G85" t="s">
+        <v>11</v>
+      </c>
+      <c r="H85" t="s">
+        <v>147</v>
+      </c>
+      <c r="I85" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>151</v>
+      </c>
+      <c r="C86" t="s">
+        <v>28</v>
+      </c>
+      <c r="D86" t="s">
+        <v>84</v>
+      </c>
+      <c r="E86" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" s="5">
+        <v>3</v>
+      </c>
+      <c r="G86" t="s">
+        <v>11</v>
+      </c>
+      <c r="H86" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>152</v>
+      </c>
+      <c r="C87" t="s">
+        <v>28</v>
+      </c>
+      <c r="D87" t="s">
+        <v>56</v>
+      </c>
+      <c r="E87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F87" s="5">
+        <v>3</v>
+      </c>
+      <c r="G87" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>153</v>
+      </c>
+      <c r="C88" t="s">
+        <v>28</v>
+      </c>
+      <c r="D88" t="s">
+        <v>56</v>
+      </c>
+      <c r="E88" t="s">
+        <v>10</v>
+      </c>
+      <c r="F88" s="5">
+        <v>3</v>
+      </c>
+      <c r="G88" t="s">
+        <v>11</v>
+      </c>
+      <c r="H88" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>154</v>
+      </c>
+      <c r="C89" t="s">
+        <v>28</v>
+      </c>
+      <c r="D89" t="s">
+        <v>84</v>
+      </c>
+      <c r="E89" t="s">
+        <v>10</v>
+      </c>
+      <c r="F89" s="5">
+        <v>3</v>
+      </c>
+      <c r="G89" t="s">
+        <v>11</v>
+      </c>
+      <c r="H89" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>155</v>
+      </c>
+      <c r="C90" t="s">
+        <v>28</v>
+      </c>
+      <c r="D90" t="s">
+        <v>125</v>
+      </c>
+      <c r="E90" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90" s="5">
+        <v>3</v>
+      </c>
+      <c r="G90" t="s">
+        <v>11</v>
+      </c>
+      <c r="H90" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>156</v>
+      </c>
+      <c r="C91" t="s">
+        <v>28</v>
+      </c>
+      <c r="D91" t="s">
+        <v>157</v>
+      </c>
+      <c r="E91" t="s">
+        <v>10</v>
+      </c>
+      <c r="F91" s="5">
+        <v>3</v>
+      </c>
+      <c r="G91" t="s">
+        <v>11</v>
+      </c>
+      <c r="H91" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2627,7 +3027,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2639,7 +3039,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2735,13 +3135,13 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0A2441A-1352-406E-94CB-A261B0FDC5B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added requirements that were missing in the spec in sections 8.3 and 12.3 and added new tests to the mapping.
</commit_message>
<xml_diff>
--- a/daffodil-core/doc/Test_Cases.xlsx
+++ b/daffodil-core/doc/Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="396" windowWidth="27792" windowHeight="11520"/>
+    <workbookView xWindow="480" yWindow="576" windowWidth="27792" windowHeight="11340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="182">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -493,6 +493,75 @@
   </si>
   <si>
     <t>DFDL-156</t>
+  </si>
+  <si>
+    <t>entity_fail_01</t>
+  </si>
+  <si>
+    <t>DFDL-6-046R</t>
+  </si>
+  <si>
+    <t>DFDL-140</t>
+  </si>
+  <si>
+    <t>entity_fail_02</t>
+  </si>
+  <si>
+    <t>entity_fail_03</t>
+  </si>
+  <si>
+    <t>entity_fail_04</t>
+  </si>
+  <si>
+    <t>byte_entities_6_01</t>
+  </si>
+  <si>
+    <t>byte_entities_6_02</t>
+  </si>
+  <si>
+    <t>byte_entities_6_03</t>
+  </si>
+  <si>
+    <t>byte_entities_6_04</t>
+  </si>
+  <si>
+    <t>byte_entities_6_05</t>
+  </si>
+  <si>
+    <t>text_entities_6_03</t>
+  </si>
+  <si>
+    <t>text_entities_6_04</t>
+  </si>
+  <si>
+    <t>DFDL-6-086R</t>
+  </si>
+  <si>
+    <t>DFDL-37</t>
+  </si>
+  <si>
+    <t>delimiter_12_04</t>
+  </si>
+  <si>
+    <t>length_explicit_12_01</t>
+  </si>
+  <si>
+    <t>DFDL-12-040R</t>
+  </si>
+  <si>
+    <t>length_explicit_12_02</t>
+  </si>
+  <si>
+    <t>text_entities_6_02</t>
+  </si>
+  <si>
+    <t>DFDL-263</t>
+  </si>
+  <si>
+    <t>NearestEnclosingSequenceElementRef</t>
+  </si>
+  <si>
+    <t>DFDL-275</t>
   </si>
 </sst>
 </file>
@@ -858,16 +927,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
-      <selection activeCell="I86" sqref="I86"/>
+    <sheetView tabSelected="1" topLeftCell="B78" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
@@ -877,7 +946,7 @@
     <col min="9" max="9" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -906,7 +975,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -929,7 +998,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -952,7 +1021,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -975,7 +1044,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>15</v>
       </c>
@@ -998,7 +1067,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>16</v>
       </c>
@@ -1021,7 +1090,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -1044,7 +1113,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -1070,7 +1139,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -1093,7 +1162,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -1119,7 +1188,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -1142,7 +1211,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>29</v>
       </c>
@@ -1168,7 +1237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -1194,7 +1263,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -1220,7 +1289,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>37</v>
       </c>
@@ -1246,7 +1315,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -1272,7 +1341,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>39</v>
       </c>
@@ -1298,7 +1367,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>41</v>
       </c>
@@ -1324,7 +1393,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>43</v>
       </c>
@@ -1350,7 +1419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>45</v>
       </c>
@@ -1373,7 +1442,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>46</v>
       </c>
@@ -1396,7 +1465,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>49</v>
       </c>
@@ -1422,7 +1491,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>50</v>
       </c>
@@ -1445,7 +1514,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>53</v>
       </c>
@@ -1468,7 +1537,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>54</v>
       </c>
@@ -1491,7 +1560,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>55</v>
       </c>
@@ -1514,7 +1583,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>57</v>
       </c>
@@ -1537,7 +1606,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>59</v>
       </c>
@@ -1560,7 +1629,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>62</v>
       </c>
@@ -1583,7 +1652,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>63</v>
       </c>
@@ -1606,7 +1675,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>64</v>
       </c>
@@ -1629,7 +1698,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>65</v>
       </c>
@@ -1652,7 +1721,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>66</v>
       </c>
@@ -1675,7 +1744,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>67</v>
       </c>
@@ -1698,7 +1767,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>68</v>
       </c>
@@ -1721,7 +1790,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>69</v>
       </c>
@@ -1744,7 +1813,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>70</v>
       </c>
@@ -1767,7 +1836,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>75</v>
       </c>
@@ -1790,7 +1859,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>76</v>
       </c>
@@ -1813,7 +1882,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>77</v>
       </c>
@@ -1836,7 +1905,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>78</v>
       </c>
@@ -1859,7 +1928,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>79</v>
       </c>
@@ -1882,7 +1951,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>82</v>
       </c>
@@ -1905,7 +1974,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>83</v>
       </c>
@@ -1928,7 +1997,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>86</v>
       </c>
@@ -1951,7 +2020,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>88</v>
       </c>
@@ -1974,7 +2043,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>90</v>
       </c>
@@ -1997,7 +2066,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>91</v>
       </c>
@@ -2020,7 +2089,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>92</v>
       </c>
@@ -2043,7 +2112,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>93</v>
       </c>
@@ -2066,7 +2135,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>94</v>
       </c>
@@ -2092,7 +2161,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>95</v>
       </c>
@@ -2115,7 +2184,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>96</v>
       </c>
@@ -2138,7 +2207,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>97</v>
       </c>
@@ -2161,7 +2230,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>100</v>
       </c>
@@ -2184,7 +2253,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>104</v>
       </c>
@@ -2207,7 +2276,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>106</v>
       </c>
@@ -2230,7 +2299,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>107</v>
       </c>
@@ -2253,7 +2322,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>109</v>
       </c>
@@ -2276,7 +2345,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>111</v>
       </c>
@@ -2299,7 +2368,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>112</v>
       </c>
@@ -2322,7 +2391,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="62" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>113</v>
       </c>
@@ -2345,7 +2414,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>114</v>
       </c>
@@ -2368,7 +2437,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="64" spans="2:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>115</v>
       </c>
@@ -2391,7 +2460,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="65" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>116</v>
       </c>
@@ -2414,7 +2483,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>118</v>
       </c>
@@ -2437,7 +2506,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>119</v>
       </c>
@@ -2460,7 +2529,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>120</v>
       </c>
@@ -2483,7 +2552,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>121</v>
       </c>
@@ -2506,7 +2575,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>122</v>
       </c>
@@ -2529,7 +2598,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>123</v>
       </c>
@@ -2552,7 +2621,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>126</v>
       </c>
@@ -2575,7 +2644,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>127</v>
       </c>
@@ -2598,7 +2667,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>128</v>
       </c>
@@ -2621,7 +2690,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="2:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>130</v>
       </c>
@@ -3013,6 +3082,386 @@
       </c>
       <c r="H91" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>159</v>
+      </c>
+      <c r="C92" t="s">
+        <v>28</v>
+      </c>
+      <c r="D92" t="s">
+        <v>160</v>
+      </c>
+      <c r="E92" t="s">
+        <v>10</v>
+      </c>
+      <c r="F92" s="5">
+        <v>3</v>
+      </c>
+      <c r="G92" t="s">
+        <v>11</v>
+      </c>
+      <c r="H92" t="s">
+        <v>161</v>
+      </c>
+      <c r="I92" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>162</v>
+      </c>
+      <c r="C93" t="s">
+        <v>28</v>
+      </c>
+      <c r="D93" t="s">
+        <v>160</v>
+      </c>
+      <c r="E93" t="s">
+        <v>10</v>
+      </c>
+      <c r="F93" s="5">
+        <v>3</v>
+      </c>
+      <c r="G93" t="s">
+        <v>11</v>
+      </c>
+      <c r="H93" t="s">
+        <v>161</v>
+      </c>
+      <c r="I93" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>163</v>
+      </c>
+      <c r="C94" t="s">
+        <v>28</v>
+      </c>
+      <c r="D94" t="s">
+        <v>160</v>
+      </c>
+      <c r="E94" t="s">
+        <v>10</v>
+      </c>
+      <c r="F94" s="5">
+        <v>3</v>
+      </c>
+      <c r="G94" t="s">
+        <v>11</v>
+      </c>
+      <c r="H94" t="s">
+        <v>161</v>
+      </c>
+      <c r="I94" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>164</v>
+      </c>
+      <c r="C95" t="s">
+        <v>28</v>
+      </c>
+      <c r="D95" t="s">
+        <v>160</v>
+      </c>
+      <c r="E95" t="s">
+        <v>10</v>
+      </c>
+      <c r="F95" s="5">
+        <v>3</v>
+      </c>
+      <c r="G95" t="s">
+        <v>11</v>
+      </c>
+      <c r="H95" t="s">
+        <v>161</v>
+      </c>
+      <c r="I95" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>165</v>
+      </c>
+      <c r="C96" t="s">
+        <v>28</v>
+      </c>
+      <c r="D96" t="s">
+        <v>101</v>
+      </c>
+      <c r="E96" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96" s="5">
+        <v>3</v>
+      </c>
+      <c r="G96" t="s">
+        <v>103</v>
+      </c>
+      <c r="H96" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>166</v>
+      </c>
+      <c r="C97" t="s">
+        <v>28</v>
+      </c>
+      <c r="D97" t="s">
+        <v>101</v>
+      </c>
+      <c r="E97" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" s="5">
+        <v>3</v>
+      </c>
+      <c r="G97" t="s">
+        <v>103</v>
+      </c>
+      <c r="H97" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>167</v>
+      </c>
+      <c r="C98" t="s">
+        <v>28</v>
+      </c>
+      <c r="D98" t="s">
+        <v>101</v>
+      </c>
+      <c r="E98" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98" s="5">
+        <v>3</v>
+      </c>
+      <c r="G98" t="s">
+        <v>103</v>
+      </c>
+      <c r="H98" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>168</v>
+      </c>
+      <c r="C99" t="s">
+        <v>28</v>
+      </c>
+      <c r="D99" t="s">
+        <v>101</v>
+      </c>
+      <c r="E99" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99" s="5">
+        <v>3</v>
+      </c>
+      <c r="G99" t="s">
+        <v>103</v>
+      </c>
+      <c r="H99" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>169</v>
+      </c>
+      <c r="C100" t="s">
+        <v>28</v>
+      </c>
+      <c r="D100" t="s">
+        <v>101</v>
+      </c>
+      <c r="E100" t="s">
+        <v>10</v>
+      </c>
+      <c r="F100" s="5">
+        <v>3</v>
+      </c>
+      <c r="G100" t="s">
+        <v>103</v>
+      </c>
+      <c r="H100" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>170</v>
+      </c>
+      <c r="C101" t="s">
+        <v>28</v>
+      </c>
+      <c r="D101" t="s">
+        <v>172</v>
+      </c>
+      <c r="E101" t="s">
+        <v>10</v>
+      </c>
+      <c r="F101" s="5">
+        <v>3</v>
+      </c>
+      <c r="G101" t="s">
+        <v>11</v>
+      </c>
+      <c r="H101" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>171</v>
+      </c>
+      <c r="C102" t="s">
+        <v>28</v>
+      </c>
+      <c r="D102" t="s">
+        <v>172</v>
+      </c>
+      <c r="E102" t="s">
+        <v>10</v>
+      </c>
+      <c r="F102" s="5">
+        <v>3</v>
+      </c>
+      <c r="G102" t="s">
+        <v>11</v>
+      </c>
+      <c r="H102" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>174</v>
+      </c>
+      <c r="C103" t="s">
+        <v>28</v>
+      </c>
+      <c r="D103" t="s">
+        <v>125</v>
+      </c>
+      <c r="E103" t="s">
+        <v>10</v>
+      </c>
+      <c r="F103" s="5">
+        <v>3</v>
+      </c>
+      <c r="G103" t="s">
+        <v>11</v>
+      </c>
+      <c r="H103" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>175</v>
+      </c>
+      <c r="C104" t="s">
+        <v>28</v>
+      </c>
+      <c r="D104" t="s">
+        <v>157</v>
+      </c>
+      <c r="E104" t="s">
+        <v>10</v>
+      </c>
+      <c r="F104" s="5">
+        <v>3</v>
+      </c>
+      <c r="G104" t="s">
+        <v>103</v>
+      </c>
+      <c r="H104" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>177</v>
+      </c>
+      <c r="C105" t="s">
+        <v>28</v>
+      </c>
+      <c r="D105" t="s">
+        <v>176</v>
+      </c>
+      <c r="E105" t="s">
+        <v>10</v>
+      </c>
+      <c r="F105" s="5">
+        <v>3</v>
+      </c>
+      <c r="G105" t="s">
+        <v>103</v>
+      </c>
+      <c r="H105" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>178</v>
+      </c>
+      <c r="C106" t="s">
+        <v>28</v>
+      </c>
+      <c r="D106" t="s">
+        <v>101</v>
+      </c>
+      <c r="E106" t="s">
+        <v>10</v>
+      </c>
+      <c r="F106" s="5">
+        <v>3</v>
+      </c>
+      <c r="G106" t="s">
+        <v>11</v>
+      </c>
+      <c r="H106" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>180</v>
+      </c>
+      <c r="C107" t="s">
+        <v>28</v>
+      </c>
+      <c r="D107" t="s">
+        <v>140</v>
+      </c>
+      <c r="E107" t="s">
+        <v>10</v>
+      </c>
+      <c r="F107" s="5">
+        <v>3</v>
+      </c>
+      <c r="G107" t="s">
+        <v>103</v>
+      </c>
+      <c r="H107" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3046,15 +3495,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000D82A129E61AB94CBD557DF296383A78" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8177165d1a918059be1ae03aa3b2f972">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -3103,6 +3543,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -3110,14 +3559,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBC5162D-F706-433F-ABDB-9F37BDA63254}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5EBC05A-E30D-4C65-8413-46397881E931}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3132,15 +3573,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBC5162D-F706-433F-ABDB-9F37BDA63254}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0A2441A-1352-406E-94CB-A261B0FDC5B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
Updates to the spreadsheets.  Tresys' tech writer had put all requirements on one sheet, Requirements-ALL sheet, in the spec so all changes should go on this sheet.  She hid the previously existing separate sheets.
</commit_message>
<xml_diff>
--- a/daffodil-core/doc/Test_Cases.xlsx
+++ b/daffodil-core/doc/Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="576" windowWidth="27792" windowHeight="11340"/>
+    <workbookView xWindow="480" yWindow="636" windowWidth="27792" windowHeight="11280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="214">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -562,6 +562,102 @@
   </si>
   <si>
     <t>DFDL-275</t>
+  </si>
+  <si>
+    <t>AR000</t>
+  </si>
+  <si>
+    <t>DFDL-17-007R</t>
+  </si>
+  <si>
+    <t>DFDL-166</t>
+  </si>
+  <si>
+    <t>AQ000</t>
+  </si>
+  <si>
+    <t>DFDL-165</t>
+  </si>
+  <si>
+    <t>AA000</t>
+  </si>
+  <si>
+    <t>DFDL-148</t>
+  </si>
+  <si>
+    <t>inputValueCalcErrorDiagnostic1</t>
+  </si>
+  <si>
+    <t>inputValueCalcErrorDiagnostic2</t>
+  </si>
+  <si>
+    <t>DelimProp_05</t>
+  </si>
+  <si>
+    <t>DFDL-271</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>AJ000</t>
+  </si>
+  <si>
+    <t>DFDL-159</t>
+  </si>
+  <si>
+    <t>AJ001</t>
+  </si>
+  <si>
+    <t>text_02</t>
+  </si>
+  <si>
+    <t>text_03</t>
+  </si>
+  <si>
+    <t>text_01</t>
+  </si>
+  <si>
+    <t>DFDL-13-235R</t>
+  </si>
+  <si>
+    <t>text_04</t>
+  </si>
+  <si>
+    <t>text_05</t>
+  </si>
+  <si>
+    <t>text_06</t>
+  </si>
+  <si>
+    <t>binary_01</t>
+  </si>
+  <si>
+    <t>entity_fail_05</t>
+  </si>
+  <si>
+    <t>entity_fail_06</t>
+  </si>
+  <si>
+    <t>property_scoping_06</t>
+  </si>
+  <si>
+    <t>DFDL-281</t>
+  </si>
+  <si>
+    <t>NumSeq_05</t>
+  </si>
+  <si>
+    <t>NumSeq_06</t>
+  </si>
+  <si>
+    <t>NumSeq_07</t>
+  </si>
+  <si>
+    <t>NumSeq_08</t>
+  </si>
+  <si>
+    <t>DFDL-63</t>
   </si>
 </sst>
 </file>
@@ -927,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B78" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="B103" workbookViewId="0">
+      <selection activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3211,7 +3307,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>166</v>
       </c>
@@ -3234,7 +3330,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>167</v>
       </c>
@@ -3257,7 +3353,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>168</v>
       </c>
@@ -3280,7 +3376,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>169</v>
       </c>
@@ -3303,7 +3399,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>170</v>
       </c>
@@ -3326,7 +3422,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>171</v>
       </c>
@@ -3349,7 +3445,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>174</v>
       </c>
@@ -3372,7 +3468,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>175</v>
       </c>
@@ -3395,7 +3491,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>177</v>
       </c>
@@ -3418,7 +3514,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>178</v>
       </c>
@@ -3432,7 +3528,7 @@
         <v>10</v>
       </c>
       <c r="F106" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G106" t="s">
         <v>11</v>
@@ -3441,7 +3537,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>180</v>
       </c>
@@ -3455,13 +3551,531 @@
         <v>10</v>
       </c>
       <c r="F107" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G107" t="s">
         <v>103</v>
       </c>
       <c r="H107" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>182</v>
+      </c>
+      <c r="C108" t="s">
+        <v>28</v>
+      </c>
+      <c r="D108" t="s">
+        <v>183</v>
+      </c>
+      <c r="E108" t="s">
+        <v>10</v>
+      </c>
+      <c r="F108" s="5">
+        <v>4</v>
+      </c>
+      <c r="G108" t="s">
+        <v>103</v>
+      </c>
+      <c r="H108" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>185</v>
+      </c>
+      <c r="C109" t="s">
+        <v>28</v>
+      </c>
+      <c r="D109" t="s">
+        <v>183</v>
+      </c>
+      <c r="E109" t="s">
+        <v>10</v>
+      </c>
+      <c r="F109" s="5">
+        <v>4</v>
+      </c>
+      <c r="G109" t="s">
+        <v>11</v>
+      </c>
+      <c r="H109" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>187</v>
+      </c>
+      <c r="C110" t="s">
+        <v>28</v>
+      </c>
+      <c r="D110" t="s">
+        <v>183</v>
+      </c>
+      <c r="E110" t="s">
+        <v>10</v>
+      </c>
+      <c r="F110" s="5">
+        <v>4</v>
+      </c>
+      <c r="G110" t="s">
+        <v>103</v>
+      </c>
+      <c r="H110" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>189</v>
+      </c>
+      <c r="C111" t="s">
+        <v>28</v>
+      </c>
+      <c r="D111" t="s">
+        <v>183</v>
+      </c>
+      <c r="E111" t="s">
+        <v>10</v>
+      </c>
+      <c r="F111" s="5">
+        <v>4</v>
+      </c>
+      <c r="G111" t="s">
+        <v>193</v>
+      </c>
+      <c r="H111" t="s">
+        <v>188</v>
+      </c>
+      <c r="I111" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>190</v>
+      </c>
+      <c r="C112" t="s">
+        <v>28</v>
+      </c>
+      <c r="D112" t="s">
+        <v>183</v>
+      </c>
+      <c r="E112" t="s">
+        <v>10</v>
+      </c>
+      <c r="F112" s="5">
+        <v>4</v>
+      </c>
+      <c r="G112" t="s">
+        <v>193</v>
+      </c>
+      <c r="H112" t="s">
+        <v>188</v>
+      </c>
+      <c r="I112" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>191</v>
+      </c>
+      <c r="C113" t="s">
+        <v>28</v>
+      </c>
+      <c r="D113" t="s">
+        <v>56</v>
+      </c>
+      <c r="E113" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113" s="5">
+        <v>4</v>
+      </c>
+      <c r="G113" t="s">
+        <v>11</v>
+      </c>
+      <c r="H113" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>194</v>
+      </c>
+      <c r="C114" t="s">
+        <v>28</v>
+      </c>
+      <c r="D114" t="s">
+        <v>105</v>
+      </c>
+      <c r="E114" t="s">
+        <v>10</v>
+      </c>
+      <c r="F114" s="5">
+        <v>4</v>
+      </c>
+      <c r="G114" t="s">
+        <v>103</v>
+      </c>
+      <c r="H114" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>196</v>
+      </c>
+      <c r="C115" t="s">
+        <v>28</v>
+      </c>
+      <c r="D115" t="s">
+        <v>105</v>
+      </c>
+      <c r="E115" t="s">
+        <v>10</v>
+      </c>
+      <c r="F115" s="5">
+        <v>4</v>
+      </c>
+      <c r="G115" t="s">
+        <v>103</v>
+      </c>
+      <c r="H115" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
+        <v>197</v>
+      </c>
+      <c r="C116" t="s">
+        <v>28</v>
+      </c>
+      <c r="D116" t="s">
+        <v>160</v>
+      </c>
+      <c r="E116" t="s">
+        <v>10</v>
+      </c>
+      <c r="F116" s="5">
+        <v>3</v>
+      </c>
+      <c r="G116" t="s">
+        <v>11</v>
+      </c>
+      <c r="H116" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>199</v>
+      </c>
+      <c r="C117" t="s">
+        <v>28</v>
+      </c>
+      <c r="D117" t="s">
+        <v>200</v>
+      </c>
+      <c r="E117" t="s">
+        <v>10</v>
+      </c>
+      <c r="F117" s="5">
+        <v>3</v>
+      </c>
+      <c r="G117" t="s">
+        <v>11</v>
+      </c>
+      <c r="H117" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>198</v>
+      </c>
+      <c r="C118" t="s">
+        <v>28</v>
+      </c>
+      <c r="D118" t="s">
+        <v>200</v>
+      </c>
+      <c r="E118" t="s">
+        <v>10</v>
+      </c>
+      <c r="F118" s="5">
+        <v>3</v>
+      </c>
+      <c r="G118" t="s">
+        <v>11</v>
+      </c>
+      <c r="H118" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>201</v>
+      </c>
+      <c r="C119" t="s">
+        <v>28</v>
+      </c>
+      <c r="D119" t="s">
+        <v>200</v>
+      </c>
+      <c r="E119" t="s">
+        <v>10</v>
+      </c>
+      <c r="F119" s="5">
+        <v>3</v>
+      </c>
+      <c r="G119" t="s">
+        <v>11</v>
+      </c>
+      <c r="H119" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>202</v>
+      </c>
+      <c r="C120" t="s">
+        <v>28</v>
+      </c>
+      <c r="D120" t="s">
+        <v>200</v>
+      </c>
+      <c r="E120" t="s">
+        <v>10</v>
+      </c>
+      <c r="F120" s="5">
+        <v>3</v>
+      </c>
+      <c r="G120" t="s">
+        <v>11</v>
+      </c>
+      <c r="H120" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>203</v>
+      </c>
+      <c r="C121" t="s">
+        <v>28</v>
+      </c>
+      <c r="D121" t="s">
+        <v>200</v>
+      </c>
+      <c r="E121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121" s="5">
+        <v>3</v>
+      </c>
+      <c r="G121" t="s">
+        <v>11</v>
+      </c>
+      <c r="H121" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>204</v>
+      </c>
+      <c r="C122" t="s">
+        <v>28</v>
+      </c>
+      <c r="D122" t="s">
+        <v>200</v>
+      </c>
+      <c r="E122" t="s">
+        <v>10</v>
+      </c>
+      <c r="F122" s="5">
+        <v>3</v>
+      </c>
+      <c r="G122" t="s">
+        <v>103</v>
+      </c>
+      <c r="H122" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>205</v>
+      </c>
+      <c r="C123" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123" t="s">
+        <v>200</v>
+      </c>
+      <c r="E123" t="s">
+        <v>10</v>
+      </c>
+      <c r="F123" s="5">
+        <v>3</v>
+      </c>
+      <c r="G123" t="s">
+        <v>103</v>
+      </c>
+      <c r="H123" t="s">
+        <v>81</v>
+      </c>
+      <c r="I123" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
+        <v>206</v>
+      </c>
+      <c r="C124" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124" t="s">
+        <v>200</v>
+      </c>
+      <c r="E124" t="s">
+        <v>10</v>
+      </c>
+      <c r="F124" s="5">
+        <v>3</v>
+      </c>
+      <c r="G124" t="s">
+        <v>103</v>
+      </c>
+      <c r="H124" t="s">
+        <v>81</v>
+      </c>
+      <c r="I124" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>207</v>
+      </c>
+      <c r="C125" t="s">
+        <v>28</v>
+      </c>
+      <c r="D125" t="s">
+        <v>140</v>
+      </c>
+      <c r="E125" t="s">
+        <v>10</v>
+      </c>
+      <c r="F125" s="5">
+        <v>4</v>
+      </c>
+      <c r="G125" t="s">
+        <v>11</v>
+      </c>
+      <c r="H125" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>209</v>
+      </c>
+      <c r="C126" t="s">
+        <v>28</v>
+      </c>
+      <c r="D126" t="s">
+        <v>51</v>
+      </c>
+      <c r="E126" t="s">
+        <v>10</v>
+      </c>
+      <c r="F126" s="5">
+        <v>4</v>
+      </c>
+      <c r="G126" t="s">
+        <v>11</v>
+      </c>
+      <c r="H126" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="127" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>210</v>
+      </c>
+      <c r="C127" t="s">
+        <v>28</v>
+      </c>
+      <c r="D127" t="s">
+        <v>51</v>
+      </c>
+      <c r="E127" t="s">
+        <v>10</v>
+      </c>
+      <c r="F127" s="5">
+        <v>4</v>
+      </c>
+      <c r="G127" t="s">
+        <v>11</v>
+      </c>
+      <c r="H127" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
+        <v>211</v>
+      </c>
+      <c r="C128" t="s">
+        <v>28</v>
+      </c>
+      <c r="D128" t="s">
+        <v>51</v>
+      </c>
+      <c r="E128" t="s">
+        <v>10</v>
+      </c>
+      <c r="F128" s="5">
+        <v>4</v>
+      </c>
+      <c r="G128" t="s">
+        <v>11</v>
+      </c>
+      <c r="H128" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>212</v>
+      </c>
+      <c r="C129" t="s">
+        <v>28</v>
+      </c>
+      <c r="D129" t="s">
+        <v>51</v>
+      </c>
+      <c r="E129" t="s">
+        <v>10</v>
+      </c>
+      <c r="F129" s="5">
+        <v>4</v>
+      </c>
+      <c r="G129" t="s">
+        <v>11</v>
+      </c>
+      <c r="H129" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -3584,10 +4198,10 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0A2441A-1352-406E-94CB-A261B0FDC5B0}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>

</xml_diff>

<commit_message>
Updated spreadsheets with new tests.
</commit_message>
<xml_diff>
--- a/daffodil-core/doc/Test_Cases.xlsx
+++ b/daffodil-core/doc/Test_Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="636" windowWidth="27792" windowHeight="11280"/>
+    <workbookView xWindow="480" yWindow="756" windowWidth="27792" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="237">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -658,6 +658,75 @@
   </si>
   <si>
     <t>DFDL-63</t>
+  </si>
+  <si>
+    <t>byte_01</t>
+  </si>
+  <si>
+    <t>inputValueCalcAbsolutePath</t>
+  </si>
+  <si>
+    <t>DFDL-283</t>
+  </si>
+  <si>
+    <t>DFDL-280</t>
+  </si>
+  <si>
+    <t>int_error_03</t>
+  </si>
+  <si>
+    <t>DFDL-279</t>
+  </si>
+  <si>
+    <t>short_02</t>
+  </si>
+  <si>
+    <t>unsignedInt_02</t>
+  </si>
+  <si>
+    <t>byte_02</t>
+  </si>
+  <si>
+    <t>unsignedByte_02</t>
+  </si>
+  <si>
+    <t>DFDL-23-011R</t>
+  </si>
+  <si>
+    <t>lke1_abs</t>
+  </si>
+  <si>
+    <t>lke1_rel</t>
+  </si>
+  <si>
+    <t>DFDL-237</t>
+  </si>
+  <si>
+    <t>ocke1</t>
+  </si>
+  <si>
+    <t>DFDL-239</t>
+  </si>
+  <si>
+    <t>ocke2</t>
+  </si>
+  <si>
+    <t>InputValueCalc_01</t>
+  </si>
+  <si>
+    <t>DFDL-236</t>
+  </si>
+  <si>
+    <t>InputValueCalc_02</t>
+  </si>
+  <si>
+    <t>InputValueCalc_03</t>
+  </si>
+  <si>
+    <t>InputValueCalc_05</t>
+  </si>
+  <si>
+    <t>InputValueCalc_06</t>
   </si>
 </sst>
 </file>
@@ -1023,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B103" workbookViewId="0">
-      <selection activeCell="F129" sqref="F129"/>
+    <sheetView tabSelected="1" topLeftCell="B120" workbookViewId="0">
+      <selection activeCell="H145" sqref="H145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3649,7 +3718,7 @@
         <v>193</v>
       </c>
       <c r="H111" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="I111" t="s">
         <v>26</v>
@@ -3675,7 +3744,7 @@
         <v>193</v>
       </c>
       <c r="H112" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
       <c r="I112" t="s">
         <v>26</v>
@@ -4055,7 +4124,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B129" t="s">
         <v>212</v>
       </c>
@@ -4076,6 +4145,398 @@
       </c>
       <c r="H129" t="s">
         <v>213</v>
+      </c>
+    </row>
+    <row r="130" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>214</v>
+      </c>
+      <c r="C130" t="s">
+        <v>28</v>
+      </c>
+      <c r="D130" t="s">
+        <v>105</v>
+      </c>
+      <c r="E130" t="s">
+        <v>10</v>
+      </c>
+      <c r="F130" s="5">
+        <v>2</v>
+      </c>
+      <c r="G130" t="s">
+        <v>11</v>
+      </c>
+      <c r="H130" t="s">
+        <v>31</v>
+      </c>
+      <c r="I130" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="131" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>215</v>
+      </c>
+      <c r="C131" t="s">
+        <v>28</v>
+      </c>
+      <c r="D131" t="s">
+        <v>183</v>
+      </c>
+      <c r="E131" t="s">
+        <v>10</v>
+      </c>
+      <c r="F131" s="5">
+        <v>4</v>
+      </c>
+      <c r="G131" t="s">
+        <v>11</v>
+      </c>
+      <c r="H131" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>218</v>
+      </c>
+      <c r="C132" t="s">
+        <v>28</v>
+      </c>
+      <c r="D132" t="s">
+        <v>17</v>
+      </c>
+      <c r="E132" t="s">
+        <v>10</v>
+      </c>
+      <c r="F132" s="5">
+        <v>4</v>
+      </c>
+      <c r="G132" t="s">
+        <v>11</v>
+      </c>
+      <c r="H132" t="s">
+        <v>219</v>
+      </c>
+      <c r="I132" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="133" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>220</v>
+      </c>
+      <c r="C133" t="s">
+        <v>28</v>
+      </c>
+      <c r="D133" t="s">
+        <v>21</v>
+      </c>
+      <c r="E133" t="s">
+        <v>10</v>
+      </c>
+      <c r="F133" s="5">
+        <v>4</v>
+      </c>
+      <c r="G133" t="s">
+        <v>11</v>
+      </c>
+      <c r="H133" t="s">
+        <v>219</v>
+      </c>
+      <c r="I133" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
+        <v>221</v>
+      </c>
+      <c r="C134" t="s">
+        <v>28</v>
+      </c>
+      <c r="D134" t="s">
+        <v>40</v>
+      </c>
+      <c r="E134" t="s">
+        <v>10</v>
+      </c>
+      <c r="F134" s="5">
+        <v>4</v>
+      </c>
+      <c r="G134" t="s">
+        <v>11</v>
+      </c>
+      <c r="H134" t="s">
+        <v>219</v>
+      </c>
+      <c r="I134" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>222</v>
+      </c>
+      <c r="C135" t="s">
+        <v>28</v>
+      </c>
+      <c r="D135" t="s">
+        <v>105</v>
+      </c>
+      <c r="E135" t="s">
+        <v>10</v>
+      </c>
+      <c r="F135" s="5">
+        <v>4</v>
+      </c>
+      <c r="G135" t="s">
+        <v>11</v>
+      </c>
+      <c r="H135" t="s">
+        <v>219</v>
+      </c>
+      <c r="I135" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>223</v>
+      </c>
+      <c r="C136" t="s">
+        <v>28</v>
+      </c>
+      <c r="D136" t="s">
+        <v>44</v>
+      </c>
+      <c r="E136" t="s">
+        <v>10</v>
+      </c>
+      <c r="F136" s="5">
+        <v>4</v>
+      </c>
+      <c r="G136" t="s">
+        <v>11</v>
+      </c>
+      <c r="H136" t="s">
+        <v>219</v>
+      </c>
+      <c r="I136" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="137" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>226</v>
+      </c>
+      <c r="C137" t="s">
+        <v>28</v>
+      </c>
+      <c r="D137" t="s">
+        <v>224</v>
+      </c>
+      <c r="E137" t="s">
+        <v>10</v>
+      </c>
+      <c r="F137" s="5">
+        <v>4</v>
+      </c>
+      <c r="G137" t="s">
+        <v>103</v>
+      </c>
+      <c r="H137" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>225</v>
+      </c>
+      <c r="C138" t="s">
+        <v>28</v>
+      </c>
+      <c r="D138" t="s">
+        <v>224</v>
+      </c>
+      <c r="E138" t="s">
+        <v>10</v>
+      </c>
+      <c r="F138" s="5">
+        <v>4</v>
+      </c>
+      <c r="G138" t="s">
+        <v>103</v>
+      </c>
+      <c r="H138" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
+        <v>228</v>
+      </c>
+      <c r="C139" t="s">
+        <v>28</v>
+      </c>
+      <c r="D139" t="s">
+        <v>224</v>
+      </c>
+      <c r="E139" t="s">
+        <v>10</v>
+      </c>
+      <c r="F139" s="5">
+        <v>4</v>
+      </c>
+      <c r="G139" t="s">
+        <v>103</v>
+      </c>
+      <c r="H139" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="140" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>230</v>
+      </c>
+      <c r="C140" t="s">
+        <v>28</v>
+      </c>
+      <c r="D140" t="s">
+        <v>224</v>
+      </c>
+      <c r="E140" t="s">
+        <v>10</v>
+      </c>
+      <c r="F140" s="5">
+        <v>4</v>
+      </c>
+      <c r="G140" t="s">
+        <v>103</v>
+      </c>
+      <c r="H140" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
+        <v>231</v>
+      </c>
+      <c r="C141" t="s">
+        <v>28</v>
+      </c>
+      <c r="D141" t="s">
+        <v>183</v>
+      </c>
+      <c r="E141" t="s">
+        <v>10</v>
+      </c>
+      <c r="F141" s="5">
+        <v>4</v>
+      </c>
+      <c r="G141" t="s">
+        <v>11</v>
+      </c>
+      <c r="H141" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="142" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
+        <v>233</v>
+      </c>
+      <c r="C142" t="s">
+        <v>28</v>
+      </c>
+      <c r="D142" t="s">
+        <v>183</v>
+      </c>
+      <c r="E142" t="s">
+        <v>10</v>
+      </c>
+      <c r="F142" s="5">
+        <v>4</v>
+      </c>
+      <c r="G142" t="s">
+        <v>11</v>
+      </c>
+      <c r="H142" t="s">
+        <v>232</v>
+      </c>
+      <c r="I142" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="143" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
+        <v>234</v>
+      </c>
+      <c r="C143" t="s">
+        <v>28</v>
+      </c>
+      <c r="D143" t="s">
+        <v>183</v>
+      </c>
+      <c r="E143" t="s">
+        <v>10</v>
+      </c>
+      <c r="F143" s="5">
+        <v>4</v>
+      </c>
+      <c r="G143" t="s">
+        <v>11</v>
+      </c>
+      <c r="H143" t="s">
+        <v>232</v>
+      </c>
+      <c r="I143" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B144" t="s">
+        <v>235</v>
+      </c>
+      <c r="C144" t="s">
+        <v>28</v>
+      </c>
+      <c r="D144" t="s">
+        <v>183</v>
+      </c>
+      <c r="E144" t="s">
+        <v>10</v>
+      </c>
+      <c r="F144" s="5">
+        <v>4</v>
+      </c>
+      <c r="G144" t="s">
+        <v>11</v>
+      </c>
+      <c r="H144" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>236</v>
+      </c>
+      <c r="C145" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" t="s">
+        <v>183</v>
+      </c>
+      <c r="E145" t="s">
+        <v>10</v>
+      </c>
+      <c r="F145" s="5">
+        <v>4</v>
+      </c>
+      <c r="G145" t="s">
+        <v>11</v>
+      </c>
+      <c r="H145" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -4109,6 +4570,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000D82A129E61AB94CBD557DF296383A78" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8177165d1a918059be1ae03aa3b2f972">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -4157,15 +4627,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -4173,6 +4634,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBC5162D-F706-433F-ABDB-9F37BDA63254}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5EBC05A-E30D-4C65-8413-46397881E931}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4183,14 +4652,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBC5162D-F706-433F-ABDB-9F37BDA63254}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>